<commit_message>
Revisão e Aaustes na formatação dos documentos
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Itens.xlsx
+++ b/planejamento/DP_Lista_Itens.xlsx
@@ -150,7 +150,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +166,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -239,18 +245,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -268,6 +274,129 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -304,133 +433,41 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="8"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -467,69 +504,45 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:I13" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:I13" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A1:I13"/>
   <sortState ref="A2:I12">
     <sortCondition ref="E1:E56"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Nome / Descrição"/>
-    <tableColumn id="2" name="Prioridade" dataDxfId="22"/>
-    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="21"/>
-    <tableColumn id="4" name="Estado Atual" dataDxfId="20"/>
-    <tableColumn id="5" name="Iteração Alvo" dataDxfId="19"/>
-    <tableColumn id="6" name="Atribuído a" dataDxfId="18"/>
-    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="17"/>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="16"/>
-    <tableColumn id="9" name="Material de Referência" dataDxfId="15"/>
+    <tableColumn id="2" name="Prioridade" dataDxfId="19"/>
+    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="18"/>
+    <tableColumn id="4" name="Estado Atual" dataDxfId="17"/>
+    <tableColumn id="5" name="Iteração Alvo" dataDxfId="16"/>
+    <tableColumn id="6" name="Atribuído a" dataDxfId="15"/>
+    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="14"/>
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="13"/>
+    <tableColumn id="9" name="Material de Referência" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabela16" displayName="Tabela16" ref="A16:I25" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A16:I25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabela16" displayName="Tabela16" ref="A16:I26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10">
+  <autoFilter ref="A16:I26"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Nome / Descrição" dataDxfId="11"/>
-    <tableColumn id="2" name="Prioridade" dataDxfId="10"/>
-    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="9"/>
-    <tableColumn id="4" name="Estado Atual" dataDxfId="8"/>
-    <tableColumn id="5" name="Iteração Alvo" dataDxfId="7"/>
-    <tableColumn id="6" name="Atribuído a" dataDxfId="6"/>
-    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="5"/>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="4"/>
-    <tableColumn id="9" name="Material de Referência" dataDxfId="3"/>
+    <tableColumn id="1" name="Nome / Descrição" dataDxfId="8"/>
+    <tableColumn id="2" name="Prioridade" dataDxfId="7"/>
+    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="6"/>
+    <tableColumn id="4" name="Estado Atual" dataDxfId="5"/>
+    <tableColumn id="5" name="Iteração Alvo" dataDxfId="4"/>
+    <tableColumn id="6" name="Atribuído a" dataDxfId="3"/>
+    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="2"/>
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="1"/>
+    <tableColumn id="9" name="Material de Referência" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -820,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A24" sqref="A1:S24"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1260,18 +1273,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="I17" s="10"/>
+    <row r="17" spans="1:9" s="14" customFormat="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="4"/>
       <c r="E18" s="4"/>
@@ -1280,7 +1295,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4"/>
       <c r="E19" s="4"/>
@@ -1289,42 +1304,42 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4"/>
       <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22"/>
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
+      <c r="G23"/>
       <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="4"/>
       <c r="E24" s="4"/>
@@ -1332,12 +1347,21 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B25" s="4"/>
-      <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="I26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Ajustes na lista de Itens e Doc. de Arquitetura
Ajustes na lista de Itens e Doc. de Arquitetura
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Itens.xlsx
+++ b/planejamento/DP_Lista_Itens.xlsx
@@ -242,9 +242,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,6 +249,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1063,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -1075,10 +1075,10 @@
         <v>29</v>
       </c>
       <c r="G8" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H8" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>28</v>
@@ -1221,28 +1221,28 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
@@ -1273,16 +1273,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="14" customFormat="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="12"/>
+    <row r="17" spans="1:9" s="13" customFormat="1">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">

</xml_diff>

<commit_message>
Ajustes, Lista de Itens
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Itens.xlsx
+++ b/planejamento/DP_Lista_Itens.xlsx
@@ -836,7 +836,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1107,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Atualização da lista de Itens
Atualização da lista de Itens
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Itens.xlsx
+++ b/planejamento/DP_Lista_Itens.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="15" windowWidth="12285" windowHeight="5910" tabRatio="457"/>
@@ -132,8 +132,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -226,16 +226,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,152 +242,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -420,53 +278,156 @@
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color indexed="8"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color indexed="8"/>
         </right>
         <top/>
         <bottom/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
-          <color indexed="8"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -492,57 +453,100 @@
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="8"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color indexed="8"/>
+          <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="8"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:I13" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:I13" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A1:I13"/>
   <sortState ref="A2:I12">
     <sortCondition ref="E1:E56"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Nome / Descrição"/>
-    <tableColumn id="2" name="Prioridade" dataDxfId="19"/>
-    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="18"/>
-    <tableColumn id="4" name="Estado Atual" dataDxfId="17"/>
-    <tableColumn id="5" name="Iteração Alvo" dataDxfId="16"/>
-    <tableColumn id="6" name="Atribuído a" dataDxfId="15"/>
-    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="14"/>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="13"/>
-    <tableColumn id="9" name="Material de Referência" dataDxfId="12"/>
+    <tableColumn id="2" name="Prioridade" dataDxfId="20"/>
+    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="19"/>
+    <tableColumn id="4" name="Estado Atual" dataDxfId="18"/>
+    <tableColumn id="5" name="Iteração Alvo" dataDxfId="17"/>
+    <tableColumn id="6" name="Atribuído a" dataDxfId="16"/>
+    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="15"/>
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="14"/>
+    <tableColumn id="9" name="Material de Referência" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabela16" displayName="Tabela16" ref="A16:I26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabela16" displayName="Tabela16" ref="A16:I26" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
   <autoFilter ref="A16:I26"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Nome / Descrição" dataDxfId="8"/>
-    <tableColumn id="2" name="Prioridade" dataDxfId="7"/>
-    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="6"/>
-    <tableColumn id="4" name="Estado Atual" dataDxfId="5"/>
-    <tableColumn id="5" name="Iteração Alvo" dataDxfId="4"/>
-    <tableColumn id="6" name="Atribuído a" dataDxfId="3"/>
-    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="2"/>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="1"/>
-    <tableColumn id="9" name="Material de Referência" dataDxfId="0"/>
+    <tableColumn id="1" name="Nome / Descrição" dataDxfId="9"/>
+    <tableColumn id="2" name="Prioridade" dataDxfId="8"/>
+    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="7"/>
+    <tableColumn id="4" name="Estado Atual" dataDxfId="6"/>
+    <tableColumn id="5" name="Iteração Alvo" dataDxfId="5"/>
+    <tableColumn id="6" name="Atribuído a" dataDxfId="4"/>
+    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="3"/>
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="2"/>
+    <tableColumn id="9" name="Material de Referência" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -623,6 +627,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -657,6 +662,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -832,14 +838,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="3" customWidth="1"/>
@@ -852,36 +858,36 @@
     <col min="9" max="9" width="38.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -910,7 +916,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -939,7 +945,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -968,7 +974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1223,114 +1229,114 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="9" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="13" customFormat="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:9">
+    <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1338,27 +1344,27 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23"/>
-      <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="I25" s="10"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
       <c r="D26" s="4"/>
@@ -1382,12 +1388,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -1396,12 +1402,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Atualizada a lista de Itens
Atualizada a lista de Itens
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Itens.xlsx
+++ b/planejamento/DP_Lista_Itens.xlsx
@@ -239,9 +239,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -251,11 +248,227 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="8"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -290,219 +503,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -514,39 +514,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:I13" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:I13" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A1:I13"/>
   <sortState ref="A2:I12">
     <sortCondition ref="E1:E56"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Nome / Descrição"/>
-    <tableColumn id="2" name="Prioridade" dataDxfId="20"/>
-    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="19"/>
-    <tableColumn id="4" name="Estado Atual" dataDxfId="18"/>
-    <tableColumn id="5" name="Iteração Alvo" dataDxfId="17"/>
-    <tableColumn id="6" name="Atribuído a" dataDxfId="16"/>
-    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="15"/>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="14"/>
-    <tableColumn id="9" name="Material de Referência" dataDxfId="13"/>
+    <tableColumn id="2" name="Prioridade" dataDxfId="19"/>
+    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="18"/>
+    <tableColumn id="4" name="Estado Atual" dataDxfId="17"/>
+    <tableColumn id="5" name="Iteração Alvo" dataDxfId="16"/>
+    <tableColumn id="6" name="Atribuído a" dataDxfId="15"/>
+    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="14"/>
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="13"/>
+    <tableColumn id="9" name="Material de Referência" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabela16" displayName="Tabela16" ref="A16:I26" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabela16" displayName="Tabela16" ref="A16:I26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10">
   <autoFilter ref="A16:I26"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Nome / Descrição" dataDxfId="9"/>
-    <tableColumn id="2" name="Prioridade" dataDxfId="8"/>
-    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="7"/>
-    <tableColumn id="4" name="Estado Atual" dataDxfId="6"/>
-    <tableColumn id="5" name="Iteração Alvo" dataDxfId="5"/>
-    <tableColumn id="6" name="Atribuído a" dataDxfId="4"/>
-    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="3"/>
-    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="2"/>
-    <tableColumn id="9" name="Material de Referência" dataDxfId="1"/>
+    <tableColumn id="1" name="Nome / Descrição" dataDxfId="8"/>
+    <tableColumn id="2" name="Prioridade" dataDxfId="7"/>
+    <tableColumn id="3" name="Tamanho Estimado (Pontos)" dataDxfId="6"/>
+    <tableColumn id="4" name="Estado Atual" dataDxfId="5"/>
+    <tableColumn id="5" name="Iteração Alvo" dataDxfId="4"/>
+    <tableColumn id="6" name="Atribuído a" dataDxfId="3"/>
+    <tableColumn id="7" name="Esforço Estimado (horas)" dataDxfId="2"/>
+    <tableColumn id="8" name="Horas Trabalhadas" dataDxfId="1"/>
+    <tableColumn id="9" name="Material de Referência" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -842,7 +842,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -858,32 +858,32 @@
     <col min="9" max="9" width="38.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1081,10 +1081,10 @@
         <v>29</v>
       </c>
       <c r="G8" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H8" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>28</v>
@@ -1230,28 +1230,28 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">

</xml_diff>

<commit_message>
Atualização da Lista Itens
Atualização da Lista Itens
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Itens.xlsx
+++ b/planejamento/DP_Lista_Itens.xlsx
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -968,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>28</v>

</xml_diff>